<commit_message>
[FMD-139] Switch DB seed to direct load from csv
+++ Load data from csv and push directly to DB.
+++ Change scope of DB fixtures
</commit_message>
<xml_diff>
--- a/tests/resources/Post_transform_EXAMPLE_data.xlsx
+++ b/tests/resources/Post_transform_EXAMPLE_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DobbsC\PycharmProjects\funding-service-design-post-award-data-store\tests\controller_tests\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SnapeN\Dev\funding-service-design-post-award-data-store\tests\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9518FE4-FABB-4B72-B03D-120720AF0FC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{696236BA-560F-481D-9AD3-2E03C42D0409}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" firstSheet="8" activeTab="15" xr2:uid="{00652EC3-4B88-41F9-B7C9-30F3C6E2549B}"/>
+    <workbookView xWindow="-30" yWindow="2730" windowWidth="28800" windowHeight="14595" firstSheet="5" activeTab="12" xr2:uid="{00652EC3-4B88-41F9-B7C9-30F3C6E2549B}"/>
   </bookViews>
   <sheets>
     <sheet name="Submission_Ref" sheetId="20" r:id="rId1"/>
@@ -1037,7 +1037,7 @@
     <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
     <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1748,14 +1748,14 @@
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>257</v>
       </c>
@@ -1769,7 +1769,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>16508</v>
       </c>
@@ -1793,16 +1793,16 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.7109375" customWidth="1"/>
     <col min="2" max="2" width="56.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -1810,7 +1810,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1818,7 +1818,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -1826,7 +1826,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -1834,7 +1834,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -1842,7 +1842,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -1850,7 +1850,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -1858,7 +1858,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -1866,7 +1866,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -1891,10 +1891,10 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.5703125" customWidth="1"/>
     <col min="2" max="2" width="24.28515625" customWidth="1"/>
@@ -1904,7 +1904,7 @@
     <col min="6" max="6" width="51.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -1924,7 +1924,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1944,7 +1944,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -1964,7 +1964,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -1984,7 +1984,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -2004,7 +2004,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -2024,7 +2024,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -2044,7 +2044,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -2064,7 +2064,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -2101,13 +2101,13 @@
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="93.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>119</v>
       </c>
@@ -2115,7 +2115,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>283</v>
       </c>
@@ -2123,7 +2123,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>284</v>
       </c>
@@ -2131,7 +2131,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>285</v>
       </c>
@@ -2139,7 +2139,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>286</v>
       </c>
@@ -2147,7 +2147,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>287</v>
       </c>
@@ -2155,7 +2155,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>288</v>
       </c>
@@ -2163,7 +2163,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>289</v>
       </c>
@@ -2171,7 +2171,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>290</v>
       </c>
@@ -2179,7 +2179,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>291</v>
       </c>
@@ -2187,7 +2187,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>292</v>
       </c>
@@ -2195,7 +2195,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>293</v>
       </c>
@@ -2203,7 +2203,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>294</v>
       </c>
@@ -2211,7 +2211,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>295</v>
       </c>
@@ -2219,7 +2219,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>296</v>
       </c>
@@ -2227,7 +2227,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>297</v>
       </c>
@@ -2235,7 +2235,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>298</v>
       </c>
@@ -2243,7 +2243,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>299</v>
       </c>
@@ -2251,7 +2251,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>300</v>
       </c>
@@ -2259,7 +2259,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>301</v>
       </c>
@@ -2267,7 +2267,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>121</v>
       </c>
@@ -2275,7 +2275,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="20" t="s">
         <v>135</v>
       </c>
@@ -2295,11 +2295,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3423617-CC86-44FD-A69A-E6E9F4D332E6}">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.42578125" customWidth="1"/>
     <col min="2" max="2" width="15.85546875" customWidth="1"/>
@@ -2311,7 +2311,7 @@
     <col min="8" max="8" width="51.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -2337,7 +2337,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -2363,7 +2363,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -2389,7 +2389,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -2415,7 +2415,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -2441,7 +2441,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -2467,7 +2467,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -2490,7 +2490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -2513,7 +2513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -2539,7 +2539,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -2565,7 +2565,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -2588,7 +2588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -2611,7 +2611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -2634,7 +2634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -2657,7 +2657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -2680,7 +2680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -2703,7 +2703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -2726,7 +2726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -2749,7 +2749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -2772,7 +2772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -2795,7 +2795,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -2818,7 +2818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -2841,7 +2841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -2864,7 +2864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -2887,7 +2887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -2910,7 +2910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -2933,7 +2933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -2956,7 +2956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>29</v>
       </c>
@@ -2979,7 +2979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -3002,7 +3002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -3025,7 +3025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -3048,7 +3048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>29</v>
       </c>
@@ -3071,7 +3071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>29</v>
       </c>
@@ -3094,7 +3094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>29</v>
       </c>
@@ -3117,7 +3117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -3140,7 +3140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>33</v>
       </c>
@@ -3163,7 +3163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>33</v>
       </c>
@@ -3186,7 +3186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>33</v>
       </c>
@@ -3209,7 +3209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>33</v>
       </c>
@@ -3232,7 +3232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>33</v>
       </c>
@@ -3255,7 +3255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>33</v>
       </c>
@@ -3278,7 +3278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>33</v>
       </c>
@@ -3301,7 +3301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>33</v>
       </c>
@@ -3324,7 +3324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>33</v>
       </c>
@@ -3347,7 +3347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>33</v>
       </c>
@@ -3385,16 +3385,16 @@
   <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="101.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>137</v>
       </c>
@@ -3402,7 +3402,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>144</v>
       </c>
@@ -3410,7 +3410,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>302</v>
       </c>
@@ -3418,7 +3418,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>145</v>
       </c>
@@ -3426,7 +3426,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>304</v>
       </c>
@@ -3434,7 +3434,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>305</v>
       </c>
@@ -3442,7 +3442,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>146</v>
       </c>
@@ -3450,7 +3450,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>147</v>
       </c>
@@ -3458,7 +3458,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>306</v>
       </c>
@@ -3466,7 +3466,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>307</v>
       </c>
@@ -3474,7 +3474,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>308</v>
       </c>
@@ -3482,7 +3482,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>148</v>
       </c>
@@ -3490,7 +3490,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>309</v>
       </c>
@@ -3498,7 +3498,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>149</v>
       </c>
@@ -3506,7 +3506,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>150</v>
       </c>
@@ -3514,7 +3514,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>151</v>
       </c>
@@ -3522,7 +3522,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>152</v>
       </c>
@@ -3530,7 +3530,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>310</v>
       </c>
@@ -3538,7 +3538,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>153</v>
       </c>
@@ -3546,7 +3546,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>311</v>
       </c>
@@ -3554,7 +3554,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>312</v>
       </c>
@@ -3562,7 +3562,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>313</v>
       </c>
@@ -3570,7 +3570,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>314</v>
       </c>
@@ -3578,7 +3578,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>315</v>
       </c>
@@ -3602,7 +3602,7 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
@@ -3616,7 +3616,7 @@
     <col min="10" max="10" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -3648,7 +3648,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -3677,7 +3677,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -3706,7 +3706,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -3735,7 +3735,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -3764,7 +3764,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -3793,7 +3793,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -3822,7 +3822,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -3851,7 +3851,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -3880,7 +3880,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -3909,7 +3909,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -3938,7 +3938,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -3967,7 +3967,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -3996,7 +3996,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -4025,7 +4025,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -4054,7 +4054,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -4080,7 +4080,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -4106,7 +4106,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -4132,7 +4132,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -4158,7 +4158,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>3</v>
       </c>
@@ -4184,7 +4184,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>3</v>
       </c>
@@ -4213,7 +4213,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>3</v>
       </c>
@@ -4242,7 +4242,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>3</v>
       </c>
@@ -4271,7 +4271,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>3</v>
       </c>
@@ -4300,7 +4300,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>3</v>
       </c>
@@ -4329,7 +4329,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="13.5" customHeight="1">
+    <row r="26" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>3</v>
       </c>
@@ -4358,7 +4358,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>3</v>
       </c>
@@ -4400,11 +4400,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3428C4CB-3892-4526-BA3F-C1E2D7B4E672}">
   <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
     <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
@@ -4421,7 +4421,7 @@
     <col min="14" max="14" width="33.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -4465,7 +4465,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -4506,7 +4506,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -4547,7 +4547,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -4588,7 +4588,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -4629,7 +4629,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -4670,7 +4670,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>3</v>
       </c>
@@ -4711,7 +4711,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -4752,7 +4752,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>3</v>
       </c>
@@ -4793,7 +4793,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" t="s">
         <v>27</v>
@@ -4835,7 +4835,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" t="s">
         <v>27</v>
@@ -4877,7 +4877,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" t="s">
         <v>27</v>
@@ -4919,7 +4919,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" t="s">
         <v>29</v>
@@ -4961,7 +4961,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" t="s">
         <v>29</v>
@@ -5003,7 +5003,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" t="s">
         <v>29</v>
@@ -5045,7 +5045,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" t="s">
         <v>33</v>
@@ -5087,7 +5087,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" t="s">
         <v>33</v>
@@ -5129,7 +5129,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" t="s">
         <v>33</v>
@@ -5171,7 +5171,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" t="s">
         <v>35</v>
@@ -5213,7 +5213,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" t="s">
         <v>35</v>
@@ -5255,7 +5255,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" t="s">
         <v>35</v>
@@ -5297,7 +5297,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" t="s">
         <v>35</v>
@@ -5339,7 +5339,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="23" spans="1:14">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" t="s">
         <v>35</v>
@@ -5381,7 +5381,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="24" spans="1:14">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" t="s">
         <v>35</v>
@@ -5423,7 +5423,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" t="s">
         <v>35</v>
@@ -5465,7 +5465,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="26" spans="1:14">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" t="s">
         <v>35</v>
@@ -5507,7 +5507,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="27" spans="1:14">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" t="s">
         <v>35</v>
@@ -5549,7 +5549,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="28" spans="1:14">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" t="s">
         <v>35</v>
@@ -5609,13 +5609,13 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -5623,7 +5623,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>271</v>
       </c>
@@ -5648,7 +5648,7 @@
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.140625" customWidth="1"/>
@@ -5656,7 +5656,7 @@
     <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5670,7 +5670,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -5699,17 +5699,17 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="113.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="59.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5720,7 +5720,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -5731,7 +5731,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -5742,7 +5742,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -5753,7 +5753,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -5764,7 +5764,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -5775,7 +5775,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -5786,7 +5786,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -5815,10 +5815,10 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="59.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.5703125" bestFit="1" customWidth="1"/>
@@ -5826,7 +5826,7 @@
     <col min="4" max="4" width="37.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -5840,7 +5840,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>41</v>
       </c>
@@ -5854,7 +5854,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -5868,7 +5868,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>46</v>
       </c>
@@ -5882,7 +5882,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>49</v>
       </c>
@@ -5896,7 +5896,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>49</v>
       </c>
@@ -5910,7 +5910,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>49</v>
       </c>
@@ -5924,7 +5924,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>55</v>
       </c>
@@ -5938,7 +5938,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>55</v>
       </c>
@@ -5952,7 +5952,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>55</v>
       </c>
@@ -5966,7 +5966,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>57</v>
       </c>
@@ -5980,7 +5980,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>57</v>
       </c>
@@ -5994,7 +5994,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>57</v>
       </c>
@@ -6008,7 +6008,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>59</v>
       </c>
@@ -6022,7 +6022,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>59</v>
       </c>
@@ -6036,7 +6036,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>59</v>
       </c>
@@ -6070,10 +6070,10 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
     <col min="2" max="2" width="82" bestFit="1" customWidth="1"/>
@@ -6082,7 +6082,7 @@
     <col min="5" max="5" width="102.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6099,7 +6099,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -6116,7 +6116,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -6133,7 +6133,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -6150,7 +6150,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -6167,7 +6167,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -6184,7 +6184,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -6201,7 +6201,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -6218,7 +6218,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -6235,7 +6235,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -6249,7 +6249,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -6263,7 +6263,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -6280,7 +6280,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -6297,7 +6297,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -6314,7 +6314,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -6331,7 +6331,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -6342,7 +6342,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -6373,7 +6373,7 @@
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="21.28515625" customWidth="1"/>
@@ -6385,7 +6385,7 @@
     <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -6414,7 +6414,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -6443,7 +6443,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -6469,7 +6469,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -6498,7 +6498,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -6524,7 +6524,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -6550,7 +6550,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -6573,7 +6573,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -6602,7 +6602,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -6628,10 +6628,10 @@
         <v>83</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" s="3"/>
     </row>
-    <row r="21" spans="4:4">
+    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D21" s="6"/>
     </row>
   </sheetData>
@@ -6649,10 +6649,10 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.85546875" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
@@ -6667,7 +6667,7 @@
     <col min="11" max="11" width="63.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -6702,7 +6702,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -6731,7 +6731,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -6758,7 +6758,7 @@
       </c>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -6787,12 +6787,12 @@
         <v>282</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="K6" s="1"/>
@@ -6815,10 +6815,10 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.42578125" customWidth="1"/>
     <col min="2" max="2" width="53.28515625" bestFit="1" customWidth="1"/>
@@ -6830,7 +6830,7 @@
     <col min="11" max="11" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -6856,7 +6856,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -6882,7 +6882,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>27</v>
       </c>
@@ -6908,7 +6908,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>27</v>
       </c>
@@ -6934,7 +6934,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>27</v>
       </c>
@@ -6960,7 +6960,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>27</v>
       </c>
@@ -6986,7 +6986,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>27</v>
       </c>
@@ -7012,7 +7012,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>27</v>
       </c>
@@ -7038,7 +7038,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>27</v>
       </c>
@@ -7064,7 +7064,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>27</v>
       </c>
@@ -7090,7 +7090,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>27</v>
       </c>
@@ -7116,7 +7116,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>27</v>
       </c>
@@ -7142,7 +7142,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>27</v>
       </c>
@@ -7168,7 +7168,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>27</v>
       </c>
@@ -7194,7 +7194,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>27</v>
       </c>
@@ -7220,36 +7220,36 @@
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G16" s="12"/>
       <c r="H16" s="12"/>
     </row>
-    <row r="17" spans="2:8">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="G17" s="12"/>
       <c r="H17" s="12"/>
     </row>
-    <row r="18" spans="2:8">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="G18" s="12"/>
       <c r="H18" s="12"/>
     </row>
-    <row r="19" spans="2:8">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="G19" s="12"/>
       <c r="H19" s="12"/>
     </row>
-    <row r="20" spans="2:8">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="13"/>
       <c r="G20" s="12"/>
       <c r="H20" s="12"/>
     </row>
-    <row r="21" spans="2:8">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="G21" s="12"/>
       <c r="H21" s="12"/>
     </row>
-    <row r="22" spans="2:8">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="G22" s="12"/>
       <c r="H22" s="12"/>
     </row>
-    <row r="23" spans="2:8">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="G23" s="12"/>
       <c r="H23" s="12"/>
     </row>
@@ -7267,6 +7267,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="681fe441-c46c-4ea5-a5c5-b45872725697">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="83a87e31-bf32-46ab-8e70-9fa18461fa4d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AB5DDB95A7ECBD49AA08D06BA3EF1CDA" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="95a99fb7649f76cf16eb4f5cafa7cbc2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="681fe441-c46c-4ea5-a5c5-b45872725697" xmlns:ns3="6bac55d2-c587-47e2-866b-bbb6fe14d104" xmlns:ns4="83a87e31-bf32-46ab-8e70-9fa18461fa4d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cbf7ff0d2c127a9a42e650b92ffbc482" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="681fe441-c46c-4ea5-a5c5-b45872725697"/>
@@ -7508,27 +7528,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70073AC4-B26C-493C-8C25-29DBD67F7B7B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="681fe441-c46c-4ea5-a5c5-b45872725697"/>
+    <ds:schemaRef ds:uri="83a87e31-bf32-46ab-8e70-9fa18461fa4d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="681fe441-c46c-4ea5-a5c5-b45872725697">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="83a87e31-bf32-46ab-8e70-9fa18461fa4d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8CA70E21-41D5-415B-B329-A133B7922149}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9931E176-D5AF-4D57-88FA-0E21DE56657D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7548,25 +7567,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8CA70E21-41D5-415B-B329-A133B7922149}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70073AC4-B26C-493C-8C25-29DBD67F7B7B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="681fe441-c46c-4ea5-a5c5-b45872725697"/>
-    <ds:schemaRef ds:uri="83a87e31-bf32-46ab-8e70-9fa18461fa4d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{95c71a0f-75e1-4c8f-90e2-641c9351dd98}" enabled="1" method="Standard" siteId="{3e0088dc-0629-4ae6-aa8c-813e7a296f50}" removed="0"/>

</xml_diff>